<commit_message>
Adicionando 3 cenarios nos artefatos
</commit_message>
<xml_diff>
--- a/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitmaapsystem\MaapSystem\artefatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Documents\MaapSystem\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44DD6E5-6BBD-42C4-AF85-5EEA220DD569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8796"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analise de Eventos" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Externo</t>
   </si>
@@ -237,11 +238,29 @@
   <si>
     <t>Analista financeiro consulta atraso dos pagamentos</t>
   </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Solicita cancelamento à fábrica</t>
+  </si>
+  <si>
+    <t>Cancela a Nota Fiscal do pedido</t>
+  </si>
+  <si>
+    <t>Cancelar Pedido</t>
+  </si>
+  <si>
+    <t>x(15)</t>
+  </si>
+  <si>
+    <t>x(16)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -874,13 +893,124 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -889,13 +1019,10 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -927,114 +1054,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1315,416 +1334,431 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="A17:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.6" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="16" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" style="16" customWidth="1"/>
-    <col min="5" max="10" width="10.6640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="2.33203125" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="16" hidden="1"/>
+    <col min="1" max="1" width="6.7109375" style="16" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="16" customWidth="1"/>
+    <col min="5" max="10" width="10.7109375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="2.28515625" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="65"/>
+      <c r="G1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="62"/>
-      <c r="I1" s="31"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="14"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+    <row r="2" spans="1:11" s="18" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65" t="s">
+      <c r="B2" s="68"/>
+      <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="H2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="65" t="s">
+      <c r="I2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="41" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="31">
         <v>1</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="70"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="54">
+    <row r="4" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="36">
         <v>2</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="72" t="s">
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="31">
         <v>3</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="44"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="50">
+    <row r="6" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="32">
         <v>4</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="76"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="50">
+    <row r="7" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="32">
         <v>5</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="75" t="s">
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="50">
+    <row r="8" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="32">
         <v>6</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="74"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="76"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="52">
+    <row r="9" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="34">
         <v>7</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="75" t="s">
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="79"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="52">
+    <row r="10" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="34">
         <v>8</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="75" t="s">
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="78"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="79"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="53"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="52">
+    <row r="11" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="58"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="34">
         <v>9</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="77"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="79"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="52">
+    <row r="12" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="58"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="34">
         <v>10</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78" t="s">
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="79"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="52">
+    <row r="13" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="34">
         <v>11</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="78" t="s">
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="79"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="52">
+    <row r="14" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="34">
         <v>12</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="79"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="53">
+    <row r="15" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="58"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="35">
         <v>13</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="78" t="s">
+      <c r="E15" s="51"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="82"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="56"/>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="54">
+    <row r="16" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="36">
         <v>14</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="73"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47"/>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+    <row r="17" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="47"/>
+      <c r="B17" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="31">
+        <v>15</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>46</v>
+      </c>
       <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="F17" s="42" t="s">
+        <v>9</v>
+      </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="J17" s="21"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
+    <row r="18" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="32">
+        <v>16</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>47</v>
+      </c>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49" t="s">
+        <v>49</v>
+      </c>
       <c r="I18" s="27"/>
       <c r="J18" s="28"/>
       <c r="K18" s="22"/>
     </row>
-    <row r="19" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
+    <row r="19" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="58"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="32">
+        <v>17</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
-      <c r="G19" s="27"/>
+      <c r="G19" s="49" t="s">
+        <v>50</v>
+      </c>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
       <c r="J19" s="28"/>
       <c r="K19" s="22"/>
     </row>
-    <row r="20" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="60"/>
+    <row r="20" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="61"/>
+      <c r="J20" s="38"/>
       <c r="K20" s="22"/>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B5:B16"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
@@ -1735,43 +1769,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:L18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="36.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="38" t="s">
+      <c r="G2" s="75"/>
+      <c r="H2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
       <c r="K2" s="1"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="78"/>
       <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
@@ -1798,12 +1832,12 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="81" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4">
@@ -1822,10 +1856,10 @@
       <c r="K4" s="11"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="4">
         <v>2</v>
       </c>
@@ -1842,7 +1876,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1856,7 +1890,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1870,7 +1904,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1884,7 +1918,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1898,7 +1932,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1912,7 +1946,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1926,7 +1960,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1940,7 +1974,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1954,7 +1988,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1968,7 +2002,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1982,7 +2016,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1996,7 +2030,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2010,7 +2044,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>

</xml_diff>

<commit_message>
Refatorou artefatos do 16 ao 19 com a atualização do DFD do terceiro cenario
</commit_message>
<xml_diff>
--- a/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Documents\MaapSystem\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44DD6E5-6BBD-42C4-AF85-5EEA220DD569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DEE100-7AB1-4D7E-9CC3-EE38DB15BCB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7995" yWindow="4275" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analise de Eventos" sheetId="1" r:id="rId1"/>
@@ -242,19 +242,19 @@
     <t>FA</t>
   </si>
   <si>
-    <t>Solicita cancelamento à fábrica</t>
-  </si>
-  <si>
-    <t>Cancela a Nota Fiscal do pedido</t>
-  </si>
-  <si>
-    <t>Cancelar Pedido</t>
-  </si>
-  <si>
     <t>x(15)</t>
   </si>
   <si>
     <t>x(16)</t>
+  </si>
+  <si>
+    <t>Loja envia solicitação de cancelamento para Departamento de vendas</t>
+  </si>
+  <si>
+    <t>Departamento Financeiro cancela pedido</t>
+  </si>
+  <si>
+    <t>Departamento Financeiro cancela NF do pedido</t>
   </si>
 </sst>
 </file>
@@ -977,6 +977,33 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
@@ -997,33 +1024,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1337,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1353,26 +1353,26 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="64" t="s">
+      <c r="F1" s="58"/>
+      <c r="G1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="65"/>
-      <c r="I1" s="66"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="14"/>
       <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" s="18" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
@@ -1400,10 +1400,10 @@
       <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="64" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="31">
@@ -1423,8 +1423,8 @@
       <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="36">
         <v>2</v>
       </c>
@@ -1442,10 +1442,10 @@
       <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="69" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="31">
@@ -1465,8 +1465,8 @@
       <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="61"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="32">
         <v>4</v>
       </c>
@@ -1484,8 +1484,8 @@
       <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="61"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="32">
         <v>5</v>
       </c>
@@ -1503,8 +1503,8 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="61"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="32">
         <v>6</v>
       </c>
@@ -1522,8 +1522,8 @@
       <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="61"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="34">
         <v>7</v>
       </c>
@@ -1541,8 +1541,8 @@
       <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="61"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="34">
         <v>8</v>
       </c>
@@ -1560,8 +1560,8 @@
       <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="61"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="34">
         <v>9</v>
       </c>
@@ -1579,8 +1579,8 @@
       <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="34">
         <v>10</v>
       </c>
@@ -1598,8 +1598,8 @@
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="34">
         <v>11</v>
       </c>
@@ -1617,8 +1617,8 @@
       <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="34">
         <v>12</v>
       </c>
@@ -1636,8 +1636,8 @@
       <c r="K14" s="22"/>
     </row>
     <row r="15" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="61"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="35">
         <v>13</v>
       </c>
@@ -1655,8 +1655,8 @@
       <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="62"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="36">
         <v>14</v>
       </c>
@@ -1674,17 +1674,17 @@
       <c r="K16" s="22"/>
     </row>
     <row r="17" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="69" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="31">
         <v>15</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="42" t="s">
@@ -1697,37 +1697,37 @@
       <c r="K17" s="22"/>
     </row>
     <row r="18" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="32">
         <v>16</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="49"/>
       <c r="H18" s="49" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="28"/>
       <c r="K18" s="22"/>
     </row>
     <row r="19" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="61"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="70"/>
       <c r="C19" s="32">
         <v>17</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="49" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
@@ -1735,8 +1735,8 @@
       <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="36"/>
       <c r="D20" s="37"/>
       <c r="E20" s="24"/>
@@ -1749,16 +1749,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A5:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refatorando artefatos de acordo com o feedback da ac4
</commit_message>
<xml_diff>
--- a/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Documents\MaapSystem\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DEE100-7AB1-4D7E-9CC3-EE38DB15BCB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70A792E-70DC-4BD1-A7D8-47612A69D209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7995" yWindow="4275" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analise de Eventos" sheetId="1" r:id="rId1"/>
@@ -188,9 +188,6 @@
     <t>Analista financeiro cobra o atraso do pagamento</t>
   </si>
   <si>
-    <t>loja recebe o boleto</t>
-  </si>
-  <si>
     <t>Analista financeiro avisa sobre o  protesto</t>
   </si>
   <si>
@@ -200,12 +197,6 @@
     <t>Banco devolve informação do ted</t>
   </si>
   <si>
-    <t>Inicia  transação com a administradora de cartões</t>
-  </si>
-  <si>
-    <t>administradora de cartões devolve transação</t>
-  </si>
-  <si>
     <t>x (2)</t>
   </si>
   <si>
@@ -255,6 +246,15 @@
   </si>
   <si>
     <t>Departamento Financeiro cancela NF do pedido</t>
+  </si>
+  <si>
+    <t>Administradora de cartões devolve transação</t>
+  </si>
+  <si>
+    <t>Loja recebe o boleto</t>
+  </si>
+  <si>
+    <t>Loja inicia transação com a administradora de cartões</t>
   </si>
 </sst>
 </file>
@@ -1337,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1434,7 @@
       <c r="E4" s="45"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
@@ -1455,7 +1455,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F5" s="45"/>
       <c r="G5" s="43"/>
@@ -1471,10 +1471,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="49"/>
@@ -1495,7 +1495,7 @@
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
       <c r="G7" s="49" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
@@ -1512,7 +1512,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F8" s="48"/>
       <c r="G8" s="49"/>
@@ -1528,7 +1528,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -1552,7 +1552,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="49" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H10" s="52"/>
       <c r="I10" s="49"/>
@@ -1566,10 +1566,10 @@
         <v>9</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="52"/>
@@ -1585,12 +1585,12 @@
         <v>10</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
       <c r="G12" s="52" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
@@ -1604,7 +1604,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -1623,10 +1623,10 @@
         <v>12</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="52"/>
@@ -1642,13 +1642,13 @@
         <v>13</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="51"/>
+        <v>50</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="54"/>
-      <c r="G15" s="52" t="s">
-        <v>18</v>
-      </c>
+      <c r="G15" s="52"/>
       <c r="H15" s="55"/>
       <c r="I15" s="55"/>
       <c r="J15" s="56"/>
@@ -1661,10 +1661,10 @@
         <v>14</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E16" s="51" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" s="45"/>
       <c r="G16" s="46"/>
@@ -1678,13 +1678,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" s="31">
         <v>15</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="42" t="s">
@@ -1703,13 +1703,13 @@
         <v>16</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="49"/>
       <c r="H18" s="49" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="28"/>
@@ -1722,12 +1722,12 @@
         <v>17</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="49" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>

</xml_diff>

<commit_message>
refatorando artefatos do 16 ao 19- feedback ac04 -eng requisitos
</commit_message>
<xml_diff>
--- a/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Documents\MaapSystem\artefatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\artefatos\MaapSystem\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70A792E-70DC-4BD1-A7D8-47612A69D209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB817983-40D3-4CF5-B99A-1D710C206899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="13188" windowHeight="11856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analise de Eventos" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Analise de Eventos'!$A$1:$J$105</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Analise de Eventos'!$A$1:$J$103</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planilha1!$A$1:$L$18</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Externo</t>
   </si>
@@ -185,12 +185,6 @@
     <t>Vendedor Gera orçamento</t>
   </si>
   <si>
-    <t>Analista financeiro cobra o atraso do pagamento</t>
-  </si>
-  <si>
-    <t>Analista financeiro avisa sobre o  protesto</t>
-  </si>
-  <si>
     <t>Inicia comunicação de consulta do ted ao banco</t>
   </si>
   <si>
@@ -209,15 +203,9 @@
     <t>x (1)</t>
   </si>
   <si>
-    <t>Loja solicita a forma de pagamento</t>
-  </si>
-  <si>
     <t>x (5)</t>
   </si>
   <si>
-    <t>x(7)</t>
-  </si>
-  <si>
     <t>x(11)</t>
   </si>
   <si>
@@ -233,12 +221,6 @@
     <t>FA</t>
   </si>
   <si>
-    <t>x(15)</t>
-  </si>
-  <si>
-    <t>x(16)</t>
-  </si>
-  <si>
     <t>Loja envia solicitação de cancelamento para Departamento de vendas</t>
   </si>
   <si>
@@ -255,6 +237,15 @@
   </si>
   <si>
     <t>Loja inicia transação com a administradora de cartões</t>
+  </si>
+  <si>
+    <t>Loja infroma a forma de pagamento</t>
+  </si>
+  <si>
+    <t>x(9)</t>
+  </si>
+  <si>
+    <t>x(14)</t>
   </si>
 </sst>
 </file>
@@ -977,6 +968,27 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1003,27 +1015,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1337,42 +1328,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.6" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="16" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="16" customWidth="1"/>
-    <col min="5" max="10" width="10.7109375" style="16" customWidth="1"/>
-    <col min="11" max="11" width="2.28515625" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="16" hidden="1"/>
+    <col min="1" max="1" width="6.6640625" style="16" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" style="16" customWidth="1"/>
+    <col min="5" max="10" width="10.6640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="2.33203125" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="57" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="57" t="s">
+      <c r="F1" s="65"/>
+      <c r="G1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="59"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="14"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+    <row r="2" spans="1:11" s="18" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="A2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="61"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
@@ -1399,11 +1390,11 @@
       </c>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+    <row r="3" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="31">
@@ -1422,9 +1413,9 @@
       <c r="J3" s="44"/>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="65"/>
+    <row r="4" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="70"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="36">
         <v>2</v>
       </c>
@@ -1434,18 +1425,18 @@
       <c r="E4" s="45"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
       <c r="J4" s="47"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+    <row r="5" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="60" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="31">
@@ -1455,7 +1446,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" s="45"/>
       <c r="G5" s="43"/>
@@ -1464,17 +1455,17 @@
       <c r="J5" s="44"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
-      <c r="B6" s="70"/>
+    <row r="6" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="58"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="32">
         <v>4</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="49"/>
@@ -1483,9 +1474,9 @@
       <c r="J6" s="50"/>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
-      <c r="B7" s="70"/>
+    <row r="7" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="58"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="32">
         <v>5</v>
       </c>
@@ -1495,16 +1486,16 @@
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
       <c r="G7" s="49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
       <c r="J7" s="50"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
-      <c r="B8" s="70"/>
+    <row r="8" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="58"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="32">
         <v>6</v>
       </c>
@@ -1512,7 +1503,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F8" s="48"/>
       <c r="G8" s="49"/>
@@ -1521,14 +1512,14 @@
       <c r="J8" s="50"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="67"/>
-      <c r="B9" s="70"/>
+    <row r="9" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="58"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="34">
         <v>7</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -1540,230 +1531,194 @@
       <c r="J9" s="53"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="67"/>
-      <c r="B10" s="70"/>
+    <row r="10" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="58"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="34">
         <v>8</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="51"/>
+        <v>43</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>36</v>
+      </c>
       <c r="F10" s="51"/>
-      <c r="G10" s="49" t="s">
-        <v>37</v>
-      </c>
+      <c r="G10" s="52"/>
       <c r="H10" s="52"/>
-      <c r="I10" s="49"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="53"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="67"/>
-      <c r="B11" s="70"/>
+    <row r="11" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="58"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="34">
         <v>9</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="51" t="s">
-        <v>40</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E11" s="51"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
+      <c r="G11" s="52" t="s">
+        <v>18</v>
+      </c>
       <c r="H11" s="52"/>
       <c r="I11" s="52"/>
       <c r="J11" s="53"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="70"/>
+    <row r="12" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="58"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="34">
         <v>10</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="51" t="s">
+        <v>46</v>
+      </c>
       <c r="F12" s="51"/>
-      <c r="G12" s="52" t="s">
-        <v>37</v>
-      </c>
+      <c r="G12" s="52"/>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
       <c r="J12" s="53"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="34">
+    <row r="13" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="58"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="35">
         <v>11</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="34">
+    <row r="14" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="59"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="36">
         <v>12</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>30</v>
+      <c r="D14" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="E14" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="22"/>
+    </row>
+    <row r="15" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="22"/>
-    </row>
-    <row r="15" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="35">
+      <c r="C15" s="31">
         <v>13</v>
       </c>
-      <c r="D15" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="54"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="56"/>
+      <c r="D15" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="36">
+    <row r="16" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="58"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="32">
         <v>14</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="47"/>
+      <c r="D16" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28"/>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="31">
+    <row r="17" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="58"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="32">
         <v>15</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="21"/>
+      <c r="D17" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="67"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="32">
-        <v>16</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="28"/>
+    <row r="18" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="59"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="38"/>
       <c r="K18" s="22"/>
     </row>
-    <row r="19" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="67"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="32">
-        <v>17</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="68"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="22"/>
-    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A5:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B5:B14"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="20" max="9" man="1"/>
+    <brk id="18" max="9" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -1776,13 +1731,13 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1"/>
       <c r="C2" s="73"/>
@@ -1800,7 +1755,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="77" t="s">
         <v>2</v>
@@ -1832,7 +1787,7 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="79" t="s">
         <v>10</v>
@@ -1856,7 +1811,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="80"/>
       <c r="C5" s="82"/>
@@ -1876,7 +1831,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1890,7 +1845,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1904,7 +1859,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1918,7 +1873,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1932,7 +1887,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1946,7 +1901,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1960,7 +1915,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1974,7 +1929,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1988,7 +1943,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2002,7 +1957,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2016,7 +1971,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2030,7 +1985,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2044,7 +1999,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>

</xml_diff>

<commit_message>
Refatorando artefatos seguindo a correção da ac5
</commit_message>
<xml_diff>
--- a/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/artefatos/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\artefatos\MaapSystem\artefatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Documents\MaapSystem\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB817983-40D3-4CF5-B99A-1D710C206899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D878FE-32B4-4FBC-A608-4BF9B562E2BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="13188" windowHeight="11856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analise de Eventos" sheetId="1" r:id="rId1"/>
@@ -239,13 +239,13 @@
     <t>Loja inicia transação com a administradora de cartões</t>
   </si>
   <si>
-    <t>Loja infroma a forma de pagamento</t>
-  </si>
-  <si>
     <t>x(9)</t>
   </si>
   <si>
     <t>x(14)</t>
+  </si>
+  <si>
+    <t>Loja informa a forma de pagamento</t>
   </si>
 </sst>
 </file>
@@ -1328,21 +1328,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.6" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="16" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" style="16" customWidth="1"/>
-    <col min="5" max="10" width="10.6640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="2.33203125" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="16" hidden="1"/>
+    <col min="1" max="1" width="6.7109375" style="16" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="16" customWidth="1"/>
+    <col min="5" max="10" width="10.7109375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="2.28515625" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="63"/>
       <c r="C1" s="63"/>
@@ -1359,7 +1359,7 @@
       <c r="J1" s="14"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="18" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
         <v>10</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="J3" s="44"/>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70"/>
       <c r="B4" s="72"/>
       <c r="C4" s="36">
@@ -1432,7 +1432,7 @@
       <c r="J4" s="47"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>11</v>
       </c>
@@ -1455,14 +1455,14 @@
       <c r="J5" s="44"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="61"/>
       <c r="C6" s="32">
         <v>4</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E6" s="48" t="s">
         <v>30</v>
@@ -1474,7 +1474,7 @@
       <c r="J6" s="50"/>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="58"/>
       <c r="B7" s="61"/>
       <c r="C7" s="32">
@@ -1493,7 +1493,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="58"/>
       <c r="B8" s="61"/>
       <c r="C8" s="32">
@@ -1512,7 +1512,7 @@
       <c r="J8" s="50"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="58"/>
       <c r="B9" s="61"/>
       <c r="C9" s="34">
@@ -1531,7 +1531,7 @@
       <c r="J9" s="53"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="58"/>
       <c r="B10" s="61"/>
       <c r="C10" s="34">
@@ -1550,7 +1550,7 @@
       <c r="J10" s="53"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
       <c r="B11" s="61"/>
       <c r="C11" s="34">
@@ -1569,7 +1569,7 @@
       <c r="J11" s="53"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58"/>
       <c r="B12" s="61"/>
       <c r="C12" s="34">
@@ -1579,7 +1579,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="52"/>
@@ -1588,7 +1588,7 @@
       <c r="J12" s="53"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>
       <c r="B13" s="61"/>
       <c r="C13" s="35">
@@ -1607,7 +1607,7 @@
       <c r="J13" s="56"/>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="59"/>
       <c r="B14" s="62"/>
       <c r="C14" s="36">
@@ -1626,7 +1626,7 @@
       <c r="J14" s="47"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="s">
         <v>17</v>
       </c>
@@ -1649,7 +1649,7 @@
       <c r="J15" s="21"/>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
       <c r="B16" s="61"/>
       <c r="C16" s="32">
@@ -1668,7 +1668,7 @@
       <c r="J16" s="28"/>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
       <c r="B17" s="61"/>
       <c r="C17" s="32">
@@ -1680,14 +1680,14 @@
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="27"/>
       <c r="J17" s="28"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11" s="23" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="23" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="59"/>
       <c r="B18" s="62"/>
       <c r="C18" s="36"/>
@@ -1700,8 +1700,8 @@
       <c r="J18" s="38"/>
       <c r="K18" s="22"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="E1:F1"/>
@@ -1731,13 +1731,13 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="36.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1"/>
       <c r="C2" s="73"/>
@@ -1755,7 +1755,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="77" t="s">
         <v>2</v>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="79" t="s">
         <v>10</v>
@@ -1811,7 +1811,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="80"/>
       <c r="C5" s="82"/>
@@ -1831,7 +1831,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1845,7 +1845,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1859,7 +1859,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1873,7 +1873,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1887,7 +1887,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1901,7 +1901,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1915,7 +1915,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1929,7 +1929,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1943,7 +1943,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1957,7 +1957,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1971,7 +1971,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1985,7 +1985,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1999,7 +1999,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>

</xml_diff>